<commit_message>
Update TIN and Address fields in Form 2307 report
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/form2307b.xlsx
+++ b/src/main/resources/excel/form2307b.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\magic\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\jchs-pos\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FE31C4-08E6-4A37-8ED9-7418D2AAF944}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31C178F-AD92-49EF-AE1F-96E26FE84E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2977,7 +2980,7 @@
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t> 001</a:t>
+            <a:t> 000</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5273,22 +5276,13 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-PH" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>160 HEROES DEL 96 ST BRGY 73</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-PH" sz="1100" baseline="0">
               <a:effectLst/>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> DIST 8 CALAANAN WEST CALOOCAN CITY</a:t>
+            <a:t>BLK 29 LOT10 EL CAMINO RD, LVDSN PEREZ, MEYCAUAYAN BULACAN</a:t>
           </a:r>
           <a:endParaRPr lang="en-PH" sz="1200">
             <a:effectLst/>
@@ -9380,11 +9374,14 @@
               <a:spcPts val="0"/>
             </a:spcAft>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200">
-            <a:effectLst/>
-            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            <a:ea typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-          </a:endParaRPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>3020</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -9658,8 +9655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="AQ17" sqref="AQ17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="AT21" sqref="AT21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Layout fix for Form 2307 To Date field
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/form2307b.xlsx
+++ b/src/main/resources/excel/form2307b.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\jchs-pos\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2496B37-9F6A-4322-ABB3-C5B1E8648B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A202A40-22B6-45E5-858A-58940E027694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3815,7 +3815,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="77276" y="530530"/>
+          <a:off x="77276" y="542722"/>
           <a:ext cx="1200714" cy="584331"/>
           <a:chOff x="7327" y="521368"/>
           <a:chExt cx="1179635" cy="669862"/>
@@ -4121,7 +4121,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1867584" y="1432450"/>
+          <a:off x="1867584" y="1446166"/>
           <a:ext cx="1014068" cy="86812"/>
           <a:chOff x="358563" y="3799299"/>
           <a:chExt cx="994293" cy="91452"/>
@@ -4407,8 +4407,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4840747" y="1291110"/>
-          <a:ext cx="1177758" cy="224059"/>
+          <a:off x="4840747" y="1301778"/>
+          <a:ext cx="1177758" cy="227107"/>
           <a:chOff x="198045" y="3663821"/>
           <a:chExt cx="1154811" cy="227822"/>
         </a:xfrm>
@@ -4889,8 +4889,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6806519" y="2610676"/>
-          <a:ext cx="338155" cy="91405"/>
+          <a:off x="6806519" y="2619820"/>
+          <a:ext cx="338155" cy="89881"/>
           <a:chOff x="3108781" y="2630100"/>
           <a:chExt cx="308840" cy="95725"/>
         </a:xfrm>
@@ -5334,7 +5334,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="6806519" y="4180379"/>
-          <a:ext cx="338155" cy="91405"/>
+          <a:ext cx="338155" cy="89881"/>
           <a:chOff x="3108781" y="2630100"/>
           <a:chExt cx="308840" cy="95725"/>
         </a:xfrm>
@@ -5497,8 +5497,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5960342" y="10474048"/>
-          <a:ext cx="1336748" cy="218615"/>
+          <a:off x="5960342" y="10422232"/>
+          <a:ext cx="1336748" cy="221663"/>
           <a:chOff x="198045" y="3663821"/>
           <a:chExt cx="1310870" cy="227822"/>
         </a:xfrm>
@@ -5932,8 +5932,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3797687" y="10474045"/>
-          <a:ext cx="1332431" cy="218616"/>
+          <a:off x="3797687" y="10422229"/>
+          <a:ext cx="1332431" cy="221664"/>
           <a:chOff x="198045" y="3663821"/>
           <a:chExt cx="1310870" cy="227822"/>
         </a:xfrm>
@@ -6437,8 +6437,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5961468" y="11525606"/>
-          <a:ext cx="1336748" cy="218617"/>
+          <a:off x="5961468" y="11470742"/>
+          <a:ext cx="1336748" cy="221665"/>
           <a:chOff x="198045" y="3663821"/>
           <a:chExt cx="1310870" cy="227822"/>
         </a:xfrm>
@@ -6872,8 +6872,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3798813" y="11525605"/>
-          <a:ext cx="1332431" cy="218617"/>
+          <a:off x="3798813" y="11470741"/>
+          <a:ext cx="1332431" cy="221665"/>
           <a:chOff x="198045" y="3663821"/>
           <a:chExt cx="1310870" cy="227822"/>
         </a:xfrm>
@@ -7378,7 +7378,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="2910481" y="3301722"/>
-          <a:ext cx="2228837" cy="218454"/>
+          <a:ext cx="2228837" cy="221502"/>
           <a:chOff x="919351" y="1740146"/>
           <a:chExt cx="2229707" cy="228603"/>
         </a:xfrm>
@@ -8052,7 +8052,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2556076" y="1718222"/>
+          <a:off x="2556076" y="1733462"/>
           <a:ext cx="2573322" cy="218749"/>
           <a:chOff x="2512808" y="1728429"/>
           <a:chExt cx="2529252" cy="217312"/>
@@ -9061,13 +9061,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>55387</xdr:colOff>
+      <xdr:colOff>36577</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>33814</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>19456</xdr:colOff>
+      <xdr:colOff>19457</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>120713</xdr:rowOff>
     </xdr:to>
@@ -9086,8 +9086,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4808970" y="1298410"/>
-          <a:ext cx="327235" cy="223086"/>
+          <a:off x="4821937" y="1301782"/>
+          <a:ext cx="348640" cy="227107"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9201,13 +9201,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>34804</xdr:colOff>
+      <xdr:colOff>22612</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>30453</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>34804</xdr:colOff>
+      <xdr:colOff>22612</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>116178</xdr:rowOff>
     </xdr:to>
@@ -9224,7 +9224,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5025904" y="1419982"/>
+          <a:off x="4990852" y="1438629"/>
           <a:ext cx="0" cy="85725"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -9655,8 +9655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="AS3" sqref="AS3"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="AU16" sqref="AU16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>